<commit_message>
marge final to main
</commit_message>
<xml_diff>
--- a/resumen_fallas_ppl.xlsx
+++ b/resumen_fallas_ppl.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B209"/>
+  <dimension ref="A1:B207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>S/NI ENTREGADO A U3449 (L3) SEGÚN SRE137 NOTA RECIBO 24/062825</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>NI ENTREGADO A U3449 (L3) SEGÚN SRE137 NOTA RECIBO 24/062825</t>
+          <t>S/NI ENTREGADO A U3449 (L3) SEGÚN SRE137 NOTA RECIBO 24/062825</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>19 F/S POR CAJA INTERCOM</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>NI ENTREGADO A U3449 (L3) SEGÚN SRE137 NOTA RECIBO 24/062825</t>
+          <t>EQ PECHO AURIC</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>19 F/S POR CAJA INTERCOM</t>
+          <t>LARINGOFONO INOPERABLES (RI MEC 7)</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>EQ PECHO AURIC</t>
+          <t>CUATRO (4) FZ F/S (ESC EXPL C BL 1)</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>LARINGOFONO INOPERABLES (RI MEC 7)</t>
+          <t>12 F/S SE190</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>CUATRO (4) FZ F/S (ESC EXPL C BL 1)</t>
+          <t>GP180 F/S</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>12 F/S SE190</t>
+          <t>CABLEADOS</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>GP180 F/S</t>
+          <t>CAJAS DE PECHO</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>CABLEADOS</t>
+          <t>AURICULARES</t>
         </is>
       </c>
     </row>
@@ -1329,31 +1329,31 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>CAJAS DE PECHO</t>
+          <t>LARINGOFONOS DEFICIENTES (RC TAN 2)</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.SEL 180/190(3W 40W)-30.A79.975MHZ-AURIC/LARI</t>
+          <t>EQUIPO DE RADIO.MAF-PHILIPS-PRC 3620-2 W-(REACONDICIONADO)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>AURICULARES</t>
+          <t>OM NRO 20/01372 NI 3336 (NO RECIBE)</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.SEL 180/190(3W 40W)-30.A79.975MHZ-AURIC/LARI</t>
+          <t>EQUIPO DE RADIO.MAF-PHILIPS-PRC 3620-2 W-(REACONDICIONADO)</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>LARINGOFONOS DEFICIENTES (RC TAN 2)</t>
+          <t>20/01373 NI 3252 (NO RECIBE) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>OM NRO 20/01372 NI 3336 (NO RECIBE)</t>
+          <t>MATERIAL CON DESGASTE</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>20/01373 NI 3252 (NO RECIBE) (ESC COM BL 1)</t>
+          <t>AVERIAS IRREPARABLES (BAL TANDIL)</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>MATERIAL CON DESGASTE</t>
+          <t>DOS (02) NO TX NO RX</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>AVERIAS IRREPARABLES (BAL TANDIL)</t>
+          <t>DOS (02) BAT BB3600 NO RETIENE CARGA (RC TAN 10)</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>DOS (02) NO TX NO RX</t>
+          <t>RT F/S</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>DOS (02) BAT BB3600 NO RETIENE CARGA (RC TAN 10)</t>
+          <t>BATERIAS F/S NO RETIENEN CARGA</t>
         </is>
       </c>
     </row>
@@ -1437,31 +1437,31 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>RT F/S</t>
+          <t>CUATRO (4) MICORTELEFONO F/S CAPSULAS DETERIORADAS (ESC ING BL 1)</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.MAF-PHILIPS-PRC 3620-2 W-(REACONDICIONADO)</t>
+          <t>EQUIPO DE RADIO.MAF-PHILIPS-VRC 3622-25W-(REACONDICIONADO)</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>BATERIAS F/S NO RETIENEN CARGA</t>
+          <t>MATERIAL CON DESGASTE</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.MAF-PHILIPS-PRC 3620-2 W-(REACONDICIONADO)</t>
+          <t>EQUIPO DE RADIO.MAF-PHILIPS-VRC 3622-25W-(REACONDICIONADO)</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>CUATRO (4) MICORTELEFONO F/S CAPSULAS DETERIORADAS (ESC ING BL 1)</t>
+          <t>AVERIAS IRREPARABLES (BAL TANDIL)</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>MATERIAL CON DESGASTE</t>
+          <t>DOS (02) REMITIDOS PARA BAJA</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>AVERIAS IRREPARABLES (BAL TANDIL)</t>
+          <t>DOS (02) NO TX NO RX (RC TAN 10)</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>DOS (02) REMITIDOS PARA BAJA</t>
+          <t>1 CABLE DE ALIMENTACIÓN NO FUNCIONA (GA BL 1)</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>DOS (02) NO TX NO RX (RC TAN 10)</t>
+          <t>TRES (3) RT F/S</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>1 CABLE DE ALIMENTACIÓN NO FUNCIONA (GA BL 1)</t>
+          <t>CABLE DE ALIMENTACION F/S (ESC ING BL 1)</t>
         </is>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>TRES (3) RT F/S</t>
+          <t>DOS (2) CABLE DE ALIMENTACON</t>
         </is>
       </c>
     </row>
@@ -1545,43 +1545,43 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>CABLE DE ALIMENTACION F/S (ESC ING BL 1)</t>
+          <t>CONECTOR CABLE DE ANTENA (JEF AGR AA EJ 601)</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.MAF-PHILIPS-VRC 3622-25W-(REACONDICIONADO)</t>
+          <t>TRANSCEPTOR.YAESU-FT 811-VEHICULAR-VHF-49 CANALES (C/PRONT)</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>DOS (2) CABLE DE ALIMENTACON</t>
+          <t>OM 20/05820 (NO ENCIENDE) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.MAF-PHILIPS-VRC 3622-25W-(REACONDICIONADO)</t>
+          <t>EQUIPO,DE COMUNICACIONES.COLLINS-DE HF-719 D/10- (SEG/PRONT)</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>CONECTOR CABLE DE ANTENA (JEF AGR AA EJ 601)</t>
+          <t>OM NRO 20/01401 NI 1138 NO SINTONIZA</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>TRANSCEPTOR.YAESU-FT 811-VEHICULAR-VHF-49 CANALES (C/PRONT)</t>
+          <t>EQUIPO,DE COMUNICACIONES.COLLINS-DE HF-719 D/10- (SEG/PRONT)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>OM 20/05820 (NO ENCIENDE) (ESC COM BL 1)</t>
+          <t>OM 22/03442 NI 1154 NO SINTONIZA</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>OM NRO 20/01401 NI 1138 NO SINTONIZA</t>
+          <t>OM 20/05821 NI 1155 NO SINTONIZA</t>
         </is>
       </c>
     </row>
@@ -1605,55 +1605,55 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>OM 22/03442 NI 1154 NO SINTONIZA</t>
+          <t>OM 22/03443 NI 1157 NO SINTONIZA (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>EQUIPO,DE COMUNICACIONES.COLLINS-DE HF-719 D/10- (SEG/PRONT)</t>
+          <t>RECEPTOR SEA 8722/A</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>OM 20/05821 NI 1155 NO SINTONIZA</t>
+          <t>UM (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>EQUIPO,DE COMUNICACIONES.COLLINS-DE HF-719 D/10- (SEG/PRONT)</t>
+          <t>TRANSCEPTOR.ICOM-IC 22 (C/PRONT)</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>OM 22/03443 NI 1157 NO SINTONIZA (ESC COM BL 1)</t>
+          <t>OM NRO 21/16755 UZ (PACK DE BATERIAS FUERA DE SERVICIO) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>RECEPTOR SEA 8722/A</t>
+          <t>EQUIPO DE RADIO.HARRIS-MPR 9600-VEHICULAR AF-C/PRONT</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>UM (ESC COM BL 1)</t>
+          <t>B00690: FALLA MODULO A4</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>TRANSCEPTOR.ICOM-IC 22 (C/PRONT)</t>
+          <t>EQUIPO DE RADIO.HARRIS-MPR 9600-VEHICULAR AF-C/PRONT</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>OM NRO 21/16755 UZ (PACK DE BATERIAS FUERA DE SERVICIO) (ESC COM BL 1)</t>
+          <t>FALLA 23. AMPLIFICADOR. 23/003/E/R</t>
         </is>
       </c>
     </row>
@@ -1665,31 +1665,31 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>B00690: FALLA MODULO A4</t>
+          <t>23/05211. REMITIDO AL BA MANT COM 601. SRE 137 NRO 23/001382. SRE 2407 23/8443(GAA MIX 602)</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.HARRIS-MPR 9600-VEHICULAR AF-C/PRONT</t>
+          <t>EQUIPO DE RADIO "MEL"UK/VRC-321</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>FALLA 23. AMPLIFICADOR. 23/003/E/R</t>
+          <t>OM NRO 22/03440 NI 275 NO SINTONIZA</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.HARRIS-MPR 9600-VEHICULAR AF-C/PRONT</t>
+          <t>EQUIPO DE RADIO "MEL"UK/VRC-321</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>23/05211. REMITIDO AL BA MANT COM 601. SRE 137 NRO 23/001382. SRE 2407 23/8443(GAA MIX 602)</t>
+          <t>OM 20/05828 NI 332 NO SINTONIZA</t>
         </is>
       </c>
     </row>
@@ -1701,43 +1701,43 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>OM NRO 22/03440 NI 275 NO SINTONIZA</t>
+          <t>OM 22/00943 NI 421 (NO ENCIENDE) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO "MEL"UK/VRC-321</t>
+          <t>TRANSCEPTOR DE VHF PRC-3000</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>OM 20/05828 NI 332 NO SINTONIZA</t>
+          <t>UM (CUENTA MUSEO) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO "MEL"UK/VRC-321</t>
+          <t>EQUIPO DE RADIO THOMPSON CSF TRC-300</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>OM 22/00943 NI 421 (NO ENCIENDE) (ESC COM BL 1)</t>
+          <t>BAT ALI 107 REMITIDO PARA MANT CANT: 4 (RC TAN 10)</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>TRANSCEPTOR DE VHF PRC-3000</t>
+          <t>EQUIPO DE RADIO THOMPSON CSF TRC-300</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>UM (CUENTA MUSEO) (ESC COM BL 1)</t>
+          <t>RT F/S</t>
         </is>
       </c>
     </row>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>BAT ALI 107 REMITIDO PARA MANT CANT: 4 (RC TAN 10)</t>
+          <t>BATERIA F/S NO RETIENE CARGA</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>RT F/S</t>
+          <t>MICROTELEFONO CAPSULAS DETERIORADAS (ESC ING BL 1)</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>BATERIA F/S NO RETIENE CARGA</t>
+          <t>CUATRO (4) F/S POR BATERÍAS (JEF AGR AA EJ 601)</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>MICROTELEFONO CAPSULAS DETERIORADAS (ESC ING BL 1)</t>
+          <t>BATERÍAS DEFICIENTE</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>CUATRO (4) F/S POR BATERÍAS (JEF AGR AA EJ 601)</t>
+          <t>EN CORTO NO ADMITEN CARGA O REPARACIÓN. PACK DE BATERÍAS 14.4V 1800MAH. NI 6371 OM 25/01913</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>BATERÍAS DEFICIENTE</t>
+          <t>NI 6398 OM 25/01314 (GAA MIX 602)</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>EN CORTO NO ADMITEN CARGA O REPARACIÓN. PACK DE BATERÍAS 14.4V 1800MAH. NI 6371 OM 25/01913</t>
+          <t>BATERÍA ALI 107 FUERA DE SERVICIO BAJO REND (RI MEC 7)</t>
         </is>
       </c>
     </row>
@@ -1833,55 +1833,55 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>NI 6398 OM 25/01314 (GAA MIX 602)</t>
+          <t>2 REMITIDAS EN B COM 601 (GAA 601)</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO THOMPSON CSF TRC-300</t>
+          <t>SWITCH D/8 PUERTOS - TP-LINK TL-SG1008</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>BATERÍA ALI 107 FUERA DE SERVICIO BAJO REND (RI MEC 7)</t>
+          <t>OM NRO 21/04690 FECHA 21/04/21 (QUEMADO) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO THOMPSON CSF TRC-300</t>
+          <t>FUENTE DE ALIMENTACION ININTERRUMPIDA.LYONN 1.2 V</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2 REMITIDAS EN B COM 601 (GAA 601)</t>
+          <t>(F/S) A DETERMINAR POR EL ESPECIALISTA (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>SWITCH D/8 PUERTOS - TP-LINK TL-SG1008</t>
+          <t>CARGADOR DE BATERIA.CR2 CN91844-CHAMPION-MULTIFUNCION-</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>OM NRO 21/04690 FECHA 21/04/21 (QUEMADO) (ESC COM BL 1)</t>
+          <t>REMITIDO AL B MANT COM 601.SRE 137 NRO 22/001319 (GAA MIX 602)</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>FUENTE DE ALIMENTACION ININTERRUMPIDA.LYONN 1.2 V</t>
+          <t>CARGADOR DE BATERIA.CR2 CN91844-CHAMPION-MULTIFUNCION-</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>(F/S) A DETERMINAR POR EL ESPECIALISTA (ESC COM BL 1)</t>
+          <t>UNO (1) NO CARGA</t>
         </is>
       </c>
     </row>
@@ -1893,211 +1893,211 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>REMITIDO AL B MANT COM 601.SRE 137 NRO 22/001319 (GAA MIX 602)</t>
+          <t>NO ENCIENDE (GAA 601)</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>CARGADOR DE BATERIA.CR2 CN91844-CHAMPION-MULTIFUNCION-</t>
+          <t>CABLE.CAMPANA ARGENTINO-PESADO COMUNICACIONES-CCA-1/PC</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>UNO (1) NO CARGA</t>
+          <t>6498 MTS (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>CARGADOR DE BATERIA.CR2 CN91844-CHAMPION-MULTIFUNCION-</t>
+          <t>CABLE TELEFONICO DE CAMPAÑA WD 1/TT</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>NO ENCIENDE (GAA 601)</t>
+          <t>8865MTS U1</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>CABLE.CAMPANA ARGENTINO-PESADO COMUNICACIONES-CCA-1/PC</t>
+          <t>CABLE TELEFONICO DE CAMPAÑA WD 1/TT</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>6498 MTS (ESC COM BL 1)</t>
+          <t>294 MTS U3 (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>CABLE TELEFONICO DE CAMPAÑA WD 1/TT</t>
+          <t>OSCILOSCOPIO PHILLIPS</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>8865MTS U1</t>
+          <t>UM (CUENTA MUSEO) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>CABLE TELEFONICO DE CAMPAÑA WD 1/TT</t>
+          <t>MULTIMETRO WESTON MOD 785</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>294 MTS U3 (ESC COM BL 1)</t>
+          <t>UM (CUENTA MUSEO) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>OSCILOSCOPIO PHILLIPS</t>
+          <t>COMPUTADORA PERSONAL.INTEL PENTIUM IV-CPO MET UNA SOLA PIEZA</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>UM (CUENTA MUSEO) (ESC COM BL 1)</t>
+          <t>OM NRO 22/06991 FECHA 19/05/22 PLACA MADRE (F/S) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>MULTIMETRO WESTON MOD 785</t>
+          <t>COMPUTADORA PERSONAL.INTEL PENTIUM IV-CPO MET UNA SOLA PIEZA</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>UM (CUENTA MUSEO) (ESC COM BL 1)</t>
+          <t>FALTA OPTIMIZAR PARA USO CORRECTO WIN10 (GA BL 1)</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>COMPUTADORA PERSONAL.INTEL PENTIUM IV-CPO MET UNA SOLA PIEZA</t>
+          <t>COMPUTADORA PERSONAL.MOD FX4300 RIGIDO-CX</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>OM NRO 22/06991 FECHA 19/05/22 PLACA MADRE (F/S) (ESC COM BL 1)</t>
+          <t>TRES (3) FALTA OPTIMIZAR PARA USO CORRECTO WIN10 (GA BL 1)</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>COMPUTADORA PERSONAL.INTEL PENTIUM IV-CPO MET UNA SOLA PIEZA</t>
+          <t>TABLET. ENDURECIDA - PX-110U - PIXART</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>FALTA OPTIMIZAR PARA USO CORRECTO WIN10 (GA BL 1)</t>
+          <t>OM NRO 24/05750 FECHA 27/05/24 UZ (BATERIA NO RETIENE CARGA) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>COMPUTADORA PERSONAL.MOD FX4300 RIGIDO-CX</t>
+          <t>MONITOR 19 TFT LCD- CDR 19WHE</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>TRES (3) FALTA OPTIMIZAR PARA USO CORRECTO WIN10 (GA BL 1)</t>
+          <t>1 F/S INOPERABLE (RC TAN 2)</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>TABLET. ENDURECIDA - PX-110U - PIXART</t>
+          <t>CABINA P/EQ RADIOENLACE DIGITAL DE CAMP. RDC C/PRONT</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>OM NRO 24/05750 FECHA 27/05/24 UZ (BATERIA NO RETIENE CARGA) (ESC COM BL 1)</t>
+          <t>ROUTER F/S REMITIDO AL B MANT COM 601</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>MONITOR 19 TFT LCD- CDR 19WHE</t>
+          <t>CABINA P/EQ RADIOENLACE DIGITAL DE CAMP. RDC C/PRONT</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>1 F/S INOPERABLE (RC TAN 2)</t>
+          <t>SRE 137 25/001611 (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>CABINA P/EQ RADIOENLACE DIGITAL DE CAMP. RDC C/PRONT</t>
+          <t>TABLET ENDURECIDA RUGGED UNRT 10</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>ROUTER F/S REMITIDO AL B MANT COM 601</t>
+          <t>(NO ENCIENDE) (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>CABINA P/EQ RADIOENLACE DIGITAL DE CAMP. RDC C/PRONT</t>
+          <t>REPETIDORA MOTOROLA MOD DGR 6175</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>SRE 137 25/001611 (ESC COM BL 1)</t>
+          <t>REMITIDA AL B MANT COM 601 SRE 137 25/001611 (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>TABLET ENDURECIDA RUGGED UNRT 10</t>
+          <t>GRUPO ELECTROGENO KIPOR MOD KDE 12 STAF</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>(NO ENCIENDE) (ESC COM BL 1)</t>
+          <t>NO ENCIENDE (ESC COM BL 1)</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>REPETIDORA MOTOROLA MOD DGR 6175</t>
+          <t>COMPUTADORA PERSONAL.(NOTEBOOK) INTEL CORE-C410</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>REMITIDA AL B MANT COM 601 SRE 137 25/001611 (ESC COM BL 1)</t>
+          <t>UNO (1) MONITOR F/S</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>GRUPO ELECTROGENO KIPOR MOD KDE 12 STAF</t>
+          <t>COMPUTADORA PERSONAL.(NOTEBOOK) INTEL CORE-C410</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>NO ENCIENDE (ESC COM BL 1)</t>
+          <t>TRES (3) BATERÍAS F/S (RC TAN 8)</t>
         </is>
       </c>
     </row>
@@ -2109,55 +2109,55 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>UNO (1) MONITOR F/S</t>
+          <t>2 ENTREGADOS PARA DISPOSICIÓN FINAL (L3) DOS(02) SRE137 NRO 21/062367 (RI MEC 7)</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>COMPUTADORA PERSONAL.(NOTEBOOK) INTEL CORE-C410</t>
+          <t>BATERIA.ALI/107-14,4 V 4 A-C/CARG C/10-P/EQ DE RADIO TRC 300</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>TRES (3) BATERÍAS F/S (RC TAN 8)</t>
+          <t>SIETE (7) CAPSULA RX</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>COMPUTADORA PERSONAL.(NOTEBOOK) INTEL CORE-C410</t>
+          <t>BATERIA.ALI/107-14,4 V 4 A-C/CARG C/10-P/EQ DE RADIO TRC 300</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>2 ENTREGADOS PARA DISPOSICIÓN FINAL (L3) DOS(02) SRE137 NRO 21/062367 (RI MEC 7)</t>
+          <t>TX DEFICIENTES (GAA MIX 602)</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>BATERIA.ALI/107-14,4 V 4 A-C/CARG C/10-P/EQ DE RADIO TRC 300</t>
+          <t>EQUIPO DE RADIO.VRC 4624-2W + 30W +IC</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>SIETE (7) CAPSULA RX</t>
+          <t>EQ PECHO COMPLETO F/S CANT: CUATRO (04) (RC TAN 10)</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>BATERIA.ALI/107-14,4 V 4 A-C/CARG C/10-P/EQ DE RADIO TRC 300</t>
+          <t>EQUIPO DE RADIO.VRC 4624-2W + 30W +IC</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>TX DEFICIENTES (GAA MIX 602)</t>
+          <t>S</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>EQ PECHO COMPLETO F/S CANT: CUATRO (04) (RC TAN 10)</t>
+          <t>2868/S</t>
         </is>
       </c>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>2709 MICROTELEFONO H189/PT</t>
         </is>
       </c>
     </row>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>2868/S</t>
+          <t>GR (01) INOPERABLE</t>
         </is>
       </c>
     </row>
@@ -2205,7 +2205,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>2709 MICROTELEFONO H189/PT</t>
+          <t>CAJA IC</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>GR (01) INOPERABLE</t>
+          <t>CABLES (01) FUERA DE SERVICIO</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>CAJA IC</t>
+          <t>ALTOPARLANTE (01) CONECTOR ROTO. S</t>
         </is>
       </c>
     </row>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>CABLES (01) FUERA DE SERVICIO</t>
+          <t>2876/S</t>
         </is>
       </c>
     </row>
@@ -2253,223 +2253,223 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>ALTOPARLANTE (01) CONECTOR ROTO. S</t>
+          <t>2798 ETAPA DE SINTONIZACIÓN INOPERABLE (RI MEC 7)</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.VRC 4624-2W + 30W +IC</t>
+          <t>TRANSCEPTOR.YAESU-FT 2600 (CONF/PRONT)</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>2876/S</t>
+          <t>NO TX NO RX CANT: UNO (01) (RC TAN 10)</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.VRC 4624-2W + 30W +IC</t>
+          <t>RADAR CORTO ALCANCE EEUU AN/PPS-15A(V)1 .045W 3KM</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>2798 ETAPA DE SINTONIZACIÓN INOPERABLE (RI MEC 7)</t>
+          <t>REMITIDO PARA MANTENIMIENTO CANT: DOS (02) (RC TAN 10)</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>TRANSCEPTOR.YAESU-FT 2600 (CONF/PRONT)</t>
+          <t>RADAR CORTO ALCANCE EEUU AN/PPS-15A(V)1 .045W 3KM</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>NO TX NO RX CANT: UNO (01) (RC TAN 10)</t>
+          <t>REMITIDO PARA MANTENIMIENTO ELON SUPERIOR SRE137 NRO 24/001515 F/S (RI MEC 7)</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>RADAR CORTO ALCANCE EEUU AN/PPS-15A(V)1 .045W 3KM</t>
+          <t>ENTRENADOR,D/TIRO.(105MM L51)TENSA-P/VC TAM-MONTADO PLATAF</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>REMITIDO PARA MANTENIMIENTO CANT: DOS (02) (RC TAN 10)</t>
+          <t>1 F/S SISTEMA ELECTRICO (RC TAN 2)</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>RADAR CORTO ALCANCE EEUU AN/PPS-15A(V)1 .045W 3KM</t>
+          <t>COMPUTADORA PERSONAL.INTEL PENTIUM IV-C/PRONT</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>REMITIDO PARA MANTENIMIENTO ELON SUPERIOR SRE137 NRO 24/001515 F/S (RI MEC 7)</t>
+          <t>PUERTOS USB F/S (RC TAN 10)</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>ENTRENADOR,D/TIRO.(105MM L51)TENSA-P/VC TAM-MONTADO PLATAF</t>
+          <t>COMPUTADORA PERSONAL.NOTEBOOK-INTEL CELERON-C/PRONT</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>1 F/S SISTEMA ELECTRICO (RC TAN 2)</t>
+          <t>BATERÍA NO RETIENE CARGA (RC TAN 10)</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>COMPUTADORA PERSONAL.INTEL PENTIUM IV-C/PRONT</t>
+          <t>COMPUTADORA NETBOOK MARCA EXO MODELO N230</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>PUERTOS USB F/S (RC TAN 10)</t>
+          <t>PLACA MOTHER QUEMADA</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>COMPUTADORA PERSONAL.NOTEBOOK-INTEL CELERON-C/PRONT</t>
+          <t>COMPUTADORA NETBOOK MARCA EXO MODELO N230</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>BATERÍA NO RETIENE CARGA (RC TAN 10)</t>
+          <t>FUENTE DE ALIMENTACIÓN QUEMADA (RI MEC 7)</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>COMPUTADORA NETBOOK MARCA EXO MODELO N230</t>
+          <t>EQUIPO DE TENDIDO RL 39/B</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>PLACA MOTHER QUEMADA</t>
+          <t>2 (DOS) MAQUINA ARROLLADORA DE CABLE F/S (GA BL 1)</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>COMPUTADORA NETBOOK MARCA EXO MODELO N230</t>
+          <t>CARGADOR DE BAT ELEC ACONCAGUA LA/501-220V P/2 BAT</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>FUENTE DE ALIMENTACIÓN QUEMADA (RI MEC 7)</t>
+          <t>DOS (2) REMITIDAS AL B COM 601 (GAA 601)</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>EQUIPO DE TENDIDO RL 39/B</t>
+          <t>EQUIPO DE NAVEGACIÓN GARMIN</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>2 (DOS) MAQUINA ARROLLADORA DE CABLE F/S (GA BL 1)</t>
+          <t>1 F/S (GA BL 1)</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>CARGADOR DE BAT ELEC ACONCAGUA LA/501-220V P/2 BAT</t>
+          <t>SIMULADOR DE TIRO AA SITARAN II</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>DOS (2) REMITIDAS AL B COM 601 (GAA 601)</t>
+          <t>FALLA EN LA PROGRAMACIÓN</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>EQUIPO DE NAVEGACIÓN GARMIN</t>
+          <t>SIMULADOR DE TIRO AA SITARAN II</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>1 F/S (GA BL 1)</t>
+          <t>SORFTWARE DESACTUALIZADO (RI MEC 7)</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>SIMULADOR DE TIRO AA SITARAN II</t>
+          <t>COMPUTADORA PERSONAL INTEL DUAL CORE</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>FALLA EN LA PROGRAMACIÓN</t>
+          <t>ONCE (11) FALTA OPTIMIZAR PARA USO CORRECTO WIN10 (GA BL 1)</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>SIMULADOR DE TIRO AA SITARAN II</t>
+          <t>COMPUTADORA PERSONAL PENTIUM 5700</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>SORFTWARE DESACTUALIZADO (RI MEC 7)</t>
+          <t>TRES (3) FALTA OPTIMIZAR PARA USO CORRECTO WIN10 (GA BL 1)</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>COMPUTADORA PERSONAL INTEL DUAL CORE</t>
+          <t>COMPUTADORA PERSONAL  (NOTEBOOK) CF 31SBLEA</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>ONCE (11) FALTA OPTIMIZAR PARA USO CORRECTO WIN10 (GA BL 1)</t>
+          <t>DOS (2) FALTA OPTIMIZAR PARA USO CORRECTO WIN10 (GA BL 1)</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>COMPUTADORA PERSONAL PENTIUM 5700</t>
+          <t>TELEFONO DE CAMPAÑA MOD TC-101</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>TRES (3) FALTA OPTIMIZAR PARA USO CORRECTO WIN10 (GA BL 1)</t>
+          <t>SEIS (6) MAGNETOS</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>COMPUTADORA PERSONAL  (NOTEBOOK) CF 31SBLEA</t>
+          <t>TELEFONO DE CAMPAÑA MOD TC-101</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>DOS (2) FALTA OPTIMIZAR PARA USO CORRECTO WIN10 (GA BL 1)</t>
+          <t>NO TRANSMITE (JEF AA EJ 601)</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>SEIS (6) MAGNETOS</t>
+          <t>OCHO (8) CAPSULA RX</t>
         </is>
       </c>
     </row>
@@ -2493,91 +2493,91 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>NO TRANSMITE (JEF AA EJ 601)</t>
+          <t>TX DEFICIENTES (GAA MIX 602)</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>TELEFONO DE CAMPAÑA MOD TC-101</t>
+          <t>TRANSCEPTOR.DE BLU-THOMSON-TRC 300/4-14,4V CC-20W</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>OCHO (8) CAPSULA RX</t>
+          <t>BATERÍAS F/S (JEF AA EJ 601)</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>TELEFONO DE CAMPAÑA MOD TC-101</t>
+          <t>TRANSCEPTOR.VHF/FM ICOM-IC V8 -(C/PRONT)</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>TX DEFICIENTES (GAA MIX 602)</t>
+          <t>BATERÍAS F/S (JEF AA EJ 601)</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>TRANSCEPTOR.DE BLU-THOMSON-TRC 300/4-14,4V CC-20W</t>
+          <t>TRANSCEPTOR.YAESU-FT 2400H-MOVIL -144 A 148MHZ- C/PRONT</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>BATERÍAS F/S (JEF AA EJ 601)</t>
+          <t>REMITIDO AL B MANT COM 601.SRE 137 NRO 23/001361</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>TRANSCEPTOR.VHF/FM ICOM-IC V8 -(C/PRONT)</t>
+          <t>TRANSCEPTOR.YAESU-FT 2400H-MOVIL -144 A 148MHZ- C/PRONT</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>BATERÍAS F/S (JEF AA EJ 601)</t>
+          <t>SRE 2407 23/8349 (GAA MIX 602)</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>TRANSCEPTOR.YAESU-FT 2400H-MOVIL -144 A 148MHZ- C/PRONT</t>
+          <t>SWITCH.DLINK-DGS 1024D</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>REMITIDO AL B MANT COM 601.SRE 137 NRO 23/001361</t>
+          <t>1 F/S INOPERABLE (RC TAN 2)</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>TRANSCEPTOR.YAESU-FT 2400H-MOVIL -144 A 148MHZ- C/PRONT</t>
+          <t>EQUIPO DE RADIO.VEHICULAR-HARRIS-RF-7800V-VS501</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>SRE 2407 23/8349 (GAA MIX 602)</t>
+          <t>MICRO TELEFONO CANT(14)</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>SWITCH.DLINK-DGS 1024D</t>
+          <t>EQUIPO DE RADIO.VEHICULAR-HARRIS-RF-7800V-VS501</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>1 F/S INOPERABLE (RC TAN 2)</t>
+          <t>STOCK MOUNT CANT(7)</t>
         </is>
       </c>
     </row>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>MICRO TELEFONO CANT(14)</t>
+          <t>EQUIPO DE PECHO CANT(3)</t>
         </is>
       </c>
     </row>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>STOCK MOUNT CANT(7)</t>
+          <t>HARRIS CANT(1)</t>
         </is>
       </c>
     </row>
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>EQUIPO DE PECHO CANT(3)</t>
+          <t>FUNDA DE TRANSPORTE CANT (1)</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>HARRIS CANT(1)</t>
+          <t>BATERÍA LITIO CANT (2)</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>FUNDA DE TRANSPORTE CANT (1)</t>
+          <t>ANTENA GPS ()CANT (1)</t>
         </is>
       </c>
     </row>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>BATERÍA LITIO CANT (2)</t>
+          <t>AMPLIFICADOR</t>
         </is>
       </c>
     </row>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>ANTENA GPS ()CANT (1)</t>
+          <t>BASE CANT (1)</t>
         </is>
       </c>
     </row>
@@ -2673,146 +2673,146 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>AMPLIFICADOR</t>
+          <t>MOCHILA CANT(2). EQUIPO DE RADIO REMITIDO AL COMPLETO (ESC EXPL C BL 1)</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.VEHICULAR-HARRIS-RF-7800V-VS501</t>
+          <t>GRUPO ELECTROGENO.ENGINE-5 KW 60 HZ-110/220V-600 A</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>BASE CANT (1)</t>
+          <t>UNO (1) SISTEMA ELECTRICO INOPERABLE (ESC EXPL C BL 1)</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>EQUIPO DE RADIO.VEHICULAR-HARRIS-RF-7800V-VS501</t>
+          <t>KIT. DE SEGURIDAD ELECTRONICA TIPO A</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>MOCHILA CANT(2). EQUIPO DE RADIO REMITIDO AL COMPLETO (ESC EXPL C BL 1)</t>
+          <t>MONITOR QUEMADO (ESC EXPL C BL 1)</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>GRUPO ELECTROGENO.ENGINE-5 KW 60 HZ-110/220V-600 A</t>
+          <t>SIMULADOR D/SISTEMAS DE ARMAS. P/MISIL TOW 2A</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>UNO (1) SISTEMA ELECTRICO INOPERABLE (ESC EXPL C BL 1)</t>
+          <t>HARDWARE</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>KIT. DE SEGURIDAD ELECTRONICA TIPO A</t>
+          <t>SIMULADOR D/SISTEMAS DE ARMAS. P/MISIL TOW 2A</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>MONITOR QUEMADO (ESC EXPL C BL 1)</t>
+          <t>SOFWARE DEFICIENTES (ESC EXPL C BL 1)</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>SIMULADOR D/SISTEMAS DE ARMAS. P/MISIL TOW 2A</t>
+          <t>CARGADOR DE BATERIA.DOLAR-12 V 100 A</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>HARDWARE</t>
+          <t>FUENTE QUEMADA (ESC EXPL C BL 1)</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>SIMULADOR D/SISTEMAS DE ARMAS. P/MISIL TOW 2A</t>
+          <t>AUTOTRANSFORMADOR DE 220/110V 50 C/S 500W</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>SOFWARE DEFICIENTES (ESC EXPL C BL 1)</t>
+          <t>UNO (1) NO ENCIENDE (GAA 601)</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>CARGADOR DE BATERIA.DOLAR-12 V 100 A</t>
+          <t>CONVERTIDOR 12/24 V 10 AMP MOD-1</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>FUENTE QUEMADA (ESC EXPL C BL 1)</t>
+          <t>DOS (2) BOBINAS DE TRASFORMADORES QUEMADAS (GAA 601)</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>AUTOTRANSFORMADOR DE 220/110V 50 C/S 500W</t>
+          <t>GRUPO ELECTROGENO WINCOLUX 105 LK-52 R-18 DE 1500W</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>UNO (1) NO ENCIENDE (GAA 601)</t>
+          <t>SISTEMA DE ALIMENTACIÓN</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>CONVERTIDOR 12/24 V 10 AMP MOD-1</t>
+          <t>GRUPO ELECTROGENO WINCOLUX 105 LK-52 R-18 DE 1500W</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>DOS (2) BOBINAS DE TRASFORMADORES QUEMADAS (GAA 601)</t>
+          <t>ENCENDIDO INOPERABLE (GAA 601)</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>GRUPO ELECTROGENO WINCOLUX 105 LK-52 R-18 DE 1500W</t>
+          <t>OSCILOSCOPIO. TEKTRONIX- TIPO 2215- DUAL-2 CANALES-C/PRONT</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>SISTEMA DE ALIMENTACIÓN</t>
+          <t>NO ADMITE REPARACIÓN (G MANT SIS AA 601)</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>GRUPO ELECTROGENO WINCOLUX 105 LK-52 R-18 DE 1500W</t>
+          <t>OSCILOSCOPIO.TEKTRONIX -P/C&amp; 35MM-C/PRONT</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>ENCENDIDO INOPERABLE (GAA 601)</t>
+          <t>NO ADMITE REPARACIÓN (G MANT SIS AA 601)</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>OSCILOSCOPIO. TEKTRONIX- TIPO 2215- DUAL-2 CANALES-C/PRONT</t>
+          <t>OSCILOSCOPIO.TEXTRONIX -465 B-DUA</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -2824,72 +2824,72 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>OSCILOSCOPIO.TEKTRONIX -P/C&amp; 35MM-C/PRONT</t>
+          <t>SIMULADOR D/TRO ARMA ANTITANQUE. RELAMPAGO-CITEFA-C/PRONT</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>NO ADMITE REPARACIÓN (G MANT SIS AA 601)</t>
+          <t>1 F/S GENERADOR INOPERABLE (RC TAN 2)</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>OSCILOSCOPIO.TEXTRONIX -465 B-DUA</t>
+          <t>ENTRENADOR DE MANEJO REPMAN-EM701- TAM/VCTP</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>NO ADMITE REPARACIÓN (G MANT SIS AA 601)</t>
+          <t>1 F/S SISTEMA ELECTRICO (RC TAN 2)</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>SIMULADOR D/TRO ARMA ANTITANQUE. RELAMPAGO-CITEFA-C/PRONT</t>
+          <t>BATERIA BB - 4600 P/EQ RADIO PRC 3620 - 4620</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>1 F/S GENERADOR INOPERABLE (RC TAN 2)</t>
+          <t>8 F/S NO RETIENEN CARGA</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>ENTRENADOR DE MANEJO REPMAN-EM701- TAM/VCTP</t>
+          <t xml:space="preserve">   KIT DE COMUNICACIONES USO EQ RADIOELECT VHF DE 2 COMPONENTES</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>1 F/S SISTEMA ELECTRICO (RC TAN 2)</t>
+          <t>8 F/S NO RETIENEN CARGA (RC TAN 2)</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>BATERIA BB - 4600 P/EQ RADIO PRC 3620 - 4620</t>
+          <t>TRANSCEPTOR HARRIS SOFT/PROGRAM Y PLAQ/GPS RF 5800-H-MP026</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>8 F/S NO RETIENEN CARGA</t>
+          <t>NI: C24015 PLACA DE CONTROL DE ALIMENTACIÓN QUEMADA (PIEZA NRO 10535</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t xml:space="preserve">   KIT DE COMUNICACIONES USO EQ RADIOELECT VHF DE 2 COMPONENTES</t>
+          <t>TRANSCEPTOR HARRIS SOFT/PROGRAM Y PLAQ/GPS RF 5800-H-MP026</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>8 F/S NO RETIENEN CARGA (RC TAN 2)</t>
+          <t>4500</t>
         </is>
       </c>
     </row>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>NI: C24015 PLACA DE CONTROL DE ALIMENTACIÓN QUEMADA (PIEZA NRO 10535</t>
+          <t>06) PLACA DE ALIMETACIÓN CON MÚLTIPLES FALLAS (PIEZA NRO: 10511</t>
         </is>
       </c>
     </row>
@@ -2912,30 +2912,6 @@
         </is>
       </c>
       <c r="B207" t="inlineStr">
-        <is>
-          <t>4500</t>
-        </is>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>TRANSCEPTOR HARRIS SOFT/PROGRAM Y PLAQ/GPS RF 5800-H-MP026</t>
-        </is>
-      </c>
-      <c r="B208" t="inlineStr">
-        <is>
-          <t>06) PLACA DE ALIMETACIÓN CON MÚLTIPLES FALLAS (PIEZA NRO: 10511</t>
-        </is>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
-        <is>
-          <t>TRANSCEPTOR HARRIS SOFT/PROGRAM Y PLAQ/GPS RF 5800-H-MP026</t>
-        </is>
-      </c>
-      <c r="B209" t="inlineStr">
         <is>
           <t>4610) (ESC ICIA BL 1)</t>
         </is>

</xml_diff>